<commit_message>
document command for /reportaa
</commit_message>
<xml_diff>
--- a/documentation/e3Commands.xlsx
+++ b/documentation/e3Commands.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="149">
   <si>
     <t xml:space="preserve">NOTE: </t>
   </si>
@@ -373,6 +373,9 @@
   </si>
   <si>
     <t>/quickburns</t>
+  </si>
+  <si>
+    <t>/reportaa</t>
   </si>
   <si>
     <t>/restock</t>
@@ -504,14 +507,15 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1060,10 +1064,10 @@
       <c r="B5" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="2" t="s">
         <v>7</v>
       </c>
       <c r="E5" t="s">
@@ -1241,7 +1245,7 @@
       <c r="A25" t="s">
         <v>47</v>
       </c>
-      <c r="E25" s="3" t="s">
+      <c r="E25" s="2" t="s">
         <v>48</v>
       </c>
     </row>
@@ -1327,7 +1331,7 @@
       <c r="B35" t="s">
         <v>43</v>
       </c>
-      <c r="E35" s="4" t="s">
+      <c r="E35" s="3" t="s">
         <v>67</v>
       </c>
     </row>
@@ -1365,7 +1369,7 @@
       <c r="A39" t="s">
         <v>73</v>
       </c>
-      <c r="E39" s="3" t="s">
+      <c r="E39" s="2" t="s">
         <v>74</v>
       </c>
     </row>
@@ -1378,7 +1382,7 @@
       </c>
     </row>
     <row r="41" ht="14.25">
-      <c r="A41" s="3" t="s">
+      <c r="A41" s="2" t="s">
         <v>77</v>
       </c>
       <c r="B41" t="s">
@@ -1452,7 +1456,7 @@
       <c r="A48" t="s">
         <v>94</v>
       </c>
-      <c r="E48" s="3" t="s">
+      <c r="E48" s="2" t="s">
         <v>95</v>
       </c>
     </row>
@@ -1493,7 +1497,7 @@
       <c r="D52" t="s">
         <v>105</v>
       </c>
-      <c r="E52" s="4" t="s">
+      <c r="E52" s="3" t="s">
         <v>106</v>
       </c>
     </row>
@@ -1536,7 +1540,7 @@
       <c r="A57" t="s">
         <v>115</v>
       </c>
-      <c r="E57" s="4" t="s">
+      <c r="E57" s="3" t="s">
         <v>116</v>
       </c>
     </row>
@@ -1549,137 +1553,143 @@
       </c>
     </row>
     <row r="59" ht="14.25">
-      <c r="A59" t="s">
+      <c r="A59" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="B59" t="s">
+      <c r="E59" s="5"/>
+    </row>
+    <row r="60" ht="14.25">
+      <c r="A60" t="s">
         <v>119</v>
       </c>
-      <c r="C59" t="s">
+      <c r="B60" t="s">
         <v>120</v>
       </c>
-      <c r="E59" t="s">
+      <c r="C60" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="60" ht="28.5">
-      <c r="A60" t="s">
+      <c r="E60" t="s">
         <v>122</v>
       </c>
-      <c r="B60" t="s">
+    </row>
+    <row r="61" ht="28.5">
+      <c r="A61" t="s">
         <v>123</v>
       </c>
-      <c r="E60" s="4" t="s">
+      <c r="B61" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="61" ht="14.25">
-      <c r="A61" t="s">
+      <c r="E61" s="3" t="s">
         <v>125</v>
-      </c>
-      <c r="E61" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="62" ht="14.25">
       <c r="A62" t="s">
+        <v>126</v>
+      </c>
+      <c r="E62" t="s">
         <v>127</v>
       </c>
-      <c r="B62" t="s">
+    </row>
+    <row r="63" ht="14.25">
+      <c r="A63" t="s">
+        <v>128</v>
+      </c>
+      <c r="B63" t="s">
         <v>84</v>
       </c>
-      <c r="E62" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="63" ht="14.25">
-      <c r="A63" s="3" t="s">
+      <c r="E63" t="s">
         <v>129</v>
       </c>
-      <c r="E63" t="s">
+    </row>
+    <row r="64" ht="14.25">
+      <c r="A64" s="2" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="64" ht="14.25">
-      <c r="A64" t="s">
+      <c r="E64" t="s">
         <v>131</v>
-      </c>
-      <c r="E64" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="65" ht="14.25">
       <c r="A65" t="s">
+        <v>132</v>
+      </c>
+      <c r="E65" t="s">
         <v>133</v>
-      </c>
-      <c r="B65" t="s">
-        <v>13</v>
-      </c>
-      <c r="E65" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="66" ht="14.25">
       <c r="A66" t="s">
+        <v>134</v>
+      </c>
+      <c r="B66" t="s">
+        <v>13</v>
+      </c>
+      <c r="E66" t="s">
         <v>135</v>
-      </c>
-      <c r="E66" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="67" ht="14.25">
       <c r="A67" t="s">
+        <v>136</v>
+      </c>
+      <c r="E67" t="s">
         <v>137</v>
-      </c>
-      <c r="E67" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="68" ht="14.25">
       <c r="A68" t="s">
+        <v>138</v>
+      </c>
+      <c r="E68" t="s">
         <v>139</v>
-      </c>
-      <c r="E68" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="69" ht="14.25">
       <c r="A69" t="s">
+        <v>140</v>
+      </c>
+      <c r="E69" t="s">
         <v>141</v>
-      </c>
-      <c r="E69" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="70" ht="14.25">
       <c r="A70" t="s">
+        <v>142</v>
+      </c>
+      <c r="E70" t="s">
         <v>143</v>
-      </c>
-      <c r="E70" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="71" ht="14.25">
       <c r="A71" t="s">
+        <v>144</v>
+      </c>
+      <c r="E71" t="s">
         <v>145</v>
-      </c>
-      <c r="E71" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="72" ht="14.25">
       <c r="A72" t="s">
+        <v>146</v>
+      </c>
+      <c r="E72" t="s">
         <v>147</v>
       </c>
-      <c r="E72" t="s">
+    </row>
+    <row r="73" ht="14.25">
+      <c r="A73" t="s">
+        <v>148</v>
+      </c>
+      <c r="E73" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="73" ht="14.25"/>
     <row r="74" ht="14.25"/>
+    <row r="75" ht="14.25"/>
   </sheetData>
-  <sortState ref="A1:A1048574" columnSort="0">
-    <sortCondition sortBy="value" descending="0" ref="A1:A1048574"/>
+  <sortState ref="A1:A1048575" columnSort="0">
+    <sortCondition sortBy="value" descending="0" ref="A1:A1048575"/>
   </sortState>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>

</xml_diff>